<commit_message>
confirmed mml phone mapping
</commit_message>
<xml_diff>
--- a/mapping/mml_phone_mapping.xlsx
+++ b/mapping/mml_phone_mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
   <si>
     <t>Elements</t>
   </si>
@@ -297,22 +297,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>structured_telecoms/country code</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>structured_telecoms/extention</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>structured_telecoms/Number</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>structured_telecoms/Area code</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>HL7 2.5</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -334,10 +318,6 @@
   </si>
   <si>
     <t>2(Telecomunication use code(Table 0201))</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>emailAddress</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -357,10 +337,6 @@
   </si>
   <si>
     <t>*memo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>*structured_telecoms/City code</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -374,15 +350,105 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Telecom type</t>
+    <t>Archetype</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>node</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_TEXT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Telecoms type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_CODED_TEXT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0001 and name/value='Telecoms']/items[at0004]/defining_code/code_string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0001 and name/value='Telecoms']/items[at0004]/defining_code/terminology_id/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_TEXT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*)値はMML0003で固定</t>
+    <rPh sb="2" eb="3">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>コテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0006]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0.21]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0007]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0019]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Structured_telecoms/Number</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Structured_telecoms/City</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Structured_telecoms/Area code</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Structured_telecoms/Extention</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sructured_telecoms/country code</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0001 and name/value='Telecoms']/items[at0002.1]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0005]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0.20]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Email address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/items[at0009 and name/value='Email address']/value</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -421,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -444,13 +510,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -474,6 +549,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -789,31 +867,30 @@
     <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="5" max="5" width="11.25" customWidth="1"/>
     <col min="8" max="8" width="26.625" customWidth="1"/>
+    <col min="9" max="9" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="W2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -830,8 +907,17 @@
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="H3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -842,8 +928,11 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="H4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -858,47 +947,41 @@
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="I5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K5" t="s">
         <v>93</v>
       </c>
-      <c r="K5">
+      <c r="W5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="H6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
@@ -908,22 +991,25 @@
         <v>12</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="H7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>94</v>
+      <c r="I7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="K7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+        <v>97</v>
+      </c>
+      <c r="W7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
@@ -933,22 +1019,25 @@
         <v>12</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="H8" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I8" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" t="s">
+        <v>98</v>
+      </c>
+      <c r="W8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
@@ -958,22 +1047,25 @@
         <v>12</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="H9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K9" t="s">
+        <v>99</v>
+      </c>
+      <c r="W9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
@@ -983,22 +1075,25 @@
         <v>12</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="H10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K10">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" t="s">
+        <v>100</v>
+      </c>
+      <c r="W10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
@@ -1008,22 +1103,25 @@
         <v>12</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="H11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" t="s">
+        <v>106</v>
+      </c>
+      <c r="W11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
@@ -1033,238 +1131,272 @@
         <v>12</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="H12" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K12">
+      <c r="I12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" t="s">
+        <v>107</v>
+      </c>
+      <c r="W12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="I13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" t="s">
+        <v>108</v>
+      </c>
+      <c r="W13">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="H13" t="s">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="I14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" t="s">
+        <v>110</v>
+      </c>
+      <c r="W14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="I15" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="H14" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="K15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B16" s="5" t="s">
+      <c r="W15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="W16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" t="s">
+      <c r="E17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" t="s">
         <v>68</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="6" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6" t="s">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B23" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B24" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B27" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B28" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B29" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B30" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
-      </c>
-      <c r="G30" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B31" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="G31" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B32" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B33" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B34" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>65</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>